<commit_message>
Additional subject and analyzeBones.m updated
</commit_message>
<xml_diff>
--- a/MATLAB/res/VSD_Subjects.xlsx
+++ b/MATLAB/res/VSD_Subjects.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AA3F83E-8C20-42AD-B62D-D64ACEC34938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6141D245-A82D-45B7-9607-7665089D708A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VSD_Subjects" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">VSD_Subjects!$B$2:$G$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">VSD_Subjects!$B$2:$G$28</definedName>
     <definedName name="Sex" comment="White cell color: Sex was checked in the CT volume. Yellow cell color: Sex was taken from the metadata.">VSD_Subjects!$D$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="49">
   <si>
     <t>F</t>
   </si>
@@ -173,6 +173,9 @@
   </si>
   <si>
     <t>019</t>
+  </si>
+  <si>
+    <t>002</t>
   </si>
 </sst>
 </file>
@@ -229,24 +232,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -587,11 +585,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:G27"/>
+  <dimension ref="B2:G28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -624,35 +620,35 @@
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="5">
+        <v>78</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>75</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1.62</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C4" s="5">
         <v>45</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E4" s="1">
         <v>54</v>
-      </c>
-      <c r="F3" s="1">
-        <v>1.65</v>
-      </c>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="7">
-        <v>30</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1">
-        <v>65</v>
       </c>
       <c r="F4" s="1">
         <v>1.65</v>
@@ -660,71 +656,71 @@
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="5">
+        <v>30</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>65</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1.65</v>
+      </c>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C6" s="5">
         <v>81</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E6" s="1">
         <v>78</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F6" s="1">
         <v>1.75</v>
       </c>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C7" s="5">
         <v>95</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E7" s="1">
         <v>60</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F7" s="1">
         <v>1.52</v>
       </c>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C8" s="5">
         <v>19</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E8" s="1">
         <v>59</v>
-      </c>
-      <c r="F7" s="1">
-        <v>1.7</v>
-      </c>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="7">
-        <v>56</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="1">
-        <v>68</v>
       </c>
       <c r="F8" s="1">
         <v>1.7</v>
@@ -732,351 +728,369 @@
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="5">
+        <v>56</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="1">
+        <v>68</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1.7</v>
+      </c>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C10" s="5">
         <v>76</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E10" s="1">
         <v>87</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F10" s="1">
         <v>1.8</v>
       </c>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C11" s="5">
         <v>25</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E11" s="1">
         <v>74</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F11" s="1">
         <v>1.75</v>
       </c>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C12" s="5">
         <v>41</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E12" s="1">
         <v>56.3</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F12" s="1">
         <v>1.65</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="6" t="s">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C13" s="5">
         <v>58</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E13" s="1">
         <v>71.3</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F13" s="1">
         <v>1.81</v>
       </c>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="6" t="s">
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C14" s="5">
         <v>47</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E14" s="1">
         <v>61</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F14" s="1">
         <v>1.66</v>
       </c>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="2:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="6" t="s">
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C15" s="5">
         <v>37</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E15" s="1">
         <v>51.5</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F15" s="1">
         <v>1.69</v>
       </c>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="6" t="s">
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C16" s="5">
         <v>30</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E16" s="1">
         <v>50.45</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F16" s="1">
         <v>1.68</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="6" t="s">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C17" s="5">
         <v>62</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D17" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="6" t="s">
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C18" s="5">
         <v>61</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E18" s="1">
         <v>53.4</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F18" s="1">
         <v>1.69</v>
       </c>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="6" t="s">
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C19" s="5">
         <v>38</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D19" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E19" s="1">
         <v>72</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F19" s="1">
         <v>1.8</v>
       </c>
-      <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="6" t="s">
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C20" s="5">
         <v>34</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D20" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E20" s="1">
         <v>87</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F20" s="1">
         <v>1.79</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="6" t="s">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C21" s="5">
         <v>84</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D21" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E21" s="1">
         <v>73.400000000000006</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F21" s="1">
         <v>1.67</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="6" t="s">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C22" s="5">
         <v>73</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D22" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E22" s="1">
         <v>73</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F22" s="1">
         <v>1.73</v>
       </c>
-      <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="6" t="s">
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="8">
+      <c r="C23" s="5">
         <v>26</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D23" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E23" s="1">
         <v>81.8</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F23" s="1">
         <v>1.87</v>
       </c>
-      <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="6" t="s">
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C24" s="5">
         <v>75</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D24" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="6" t="s">
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="8">
+      <c r="C25" s="5">
         <v>39</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D25" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E25" s="1">
         <v>37.4</v>
       </c>
-      <c r="F24" s="1">
+      <c r="F25" s="1">
         <v>1.8</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="6" t="s">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="8">
+      <c r="C26" s="5">
         <v>43</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D26" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E26" s="1">
         <v>76.95</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F26" s="1">
         <v>1.77</v>
       </c>
-      <c r="G25" s="1"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="6" t="s">
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="8">
+      <c r="C27" s="5">
         <v>69</v>
       </c>
-      <c r="D26" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C27" s="8">
-        <v>48</v>
-      </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-      <c r="G27" s="1" t="s">
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="5">
+        <v>48</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B2:G27" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:G27">
-      <sortCondition ref="B2:B27"/>
+  <autoFilter ref="B2:G28" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:G28">
+      <sortCondition ref="B2:B28"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B9:G27">
-    <sortCondition ref="B9:B18"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B10:G28">
+    <sortCondition ref="B10:B19"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Additional subjects added. Fixes of intersections of adjacent bones.
</commit_message>
<xml_diff>
--- a/MATLAB/res/VSD_Subjects.xlsx
+++ b/MATLAB/res/VSD_Subjects.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6141D245-A82D-45B7-9607-7665089D708A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E71F7F54-90E6-4169-90EB-6B07974D7055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VSD_Subjects" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">VSD_Subjects!$B$2:$G$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">VSD_Subjects!$B$2:$G$30</definedName>
     <definedName name="Sex" comment="White cell color: Sex was checked in the CT volume. Yellow cell color: Sex was taken from the metadata.">VSD_Subjects!$D$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -29,14 +29,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="52">
   <si>
     <t>F</t>
   </si>
   <si>
-    <t>Number</t>
-  </si>
-  <si>
     <t>z001</t>
   </si>
   <si>
@@ -139,15 +136,9 @@
     <t>Comment</t>
   </si>
   <si>
-    <t>Dupe of z30</t>
-  </si>
-  <si>
     <t>010</t>
   </si>
   <si>
-    <t>Dupe of z024, intraosseous access left tibia</t>
-  </si>
-  <si>
     <t>014</t>
   </si>
   <si>
@@ -157,18 +148,6 @@
     <t>017</t>
   </si>
   <si>
-    <t>In the metadata the subject is incorrectly defined as female</t>
-  </si>
-  <si>
-    <t>Right phalanges are cut off</t>
-  </si>
-  <si>
-    <t>Dupe of z11, hinged total knee replacement of the right knee joint</t>
-  </si>
-  <si>
-    <t>Metal artifacts, Metacarpals are cut off and phalanges are missing</t>
-  </si>
-  <si>
     <t>015</t>
   </si>
   <si>
@@ -176,6 +155,36 @@
   </si>
   <si>
     <t>002</t>
+  </si>
+  <si>
+    <t>z004</t>
+  </si>
+  <si>
+    <t>006</t>
+  </si>
+  <si>
+    <t>Missing body weight and height.</t>
+  </si>
+  <si>
+    <t>Metacarpals are cut off and phalanges are missing. Metal artifacts.</t>
+  </si>
+  <si>
+    <t>In the meta data the subject is incorrectly defined as female.</t>
+  </si>
+  <si>
+    <t>Dupe of VSD z011. Hinged total knee replacement of the right knee joint.</t>
+  </si>
+  <si>
+    <t>Dupe of VSD z030.</t>
+  </si>
+  <si>
+    <t>Right phalanges are cut off.</t>
+  </si>
+  <si>
+    <t>Dupe of VSD z024 with conflicting meta data. Intraosseous access in the left tibia.</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -585,7 +594,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:G28"/>
+  <dimension ref="B2:G30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -601,27 +610,27 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="E2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C3" s="5">
         <v>78</v>
@@ -639,34 +648,34 @@
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C4" s="5">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="1">
-        <v>54</v>
+        <v>90</v>
       </c>
       <c r="F4" s="1">
-        <v>1.65</v>
+        <v>1.77</v>
       </c>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C5" s="5">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="1">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="F5" s="1">
         <v>1.65</v>
@@ -675,70 +684,70 @@
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C6" s="5">
-        <v>81</v>
+        <v>30</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="E6" s="1">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="F6" s="1">
-        <v>1.75</v>
+        <v>1.65</v>
       </c>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" s="5">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="E7" s="1">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="F7" s="1">
-        <v>1.52</v>
+        <v>1.75</v>
       </c>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C8" s="5">
-        <v>19</v>
+        <v>95</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="1">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F8" s="1">
-        <v>1.7</v>
+        <v>1.52</v>
       </c>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C9" s="5">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="E9" s="1">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="F9" s="1">
         <v>1.7</v>
@@ -746,353 +755,398 @@
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
-        <v>2</v>
+      <c r="B10" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="C10" s="5">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E10" s="1">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="F10" s="1">
-        <v>1.8</v>
+        <v>1.7</v>
       </c>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C11" s="5">
-        <v>25</v>
+        <v>76</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E11" s="1">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="F11" s="1">
-        <v>1.75</v>
+        <v>1.8</v>
       </c>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="C12" s="5">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E12" s="1">
-        <v>56.3</v>
+        <v>82.3</v>
       </c>
       <c r="F12" s="1">
-        <v>1.65</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>1.77</v>
+      </c>
+      <c r="G12" s="1"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C13" s="5">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E13" s="1">
-        <v>71.3</v>
+        <v>74</v>
       </c>
       <c r="F13" s="1">
-        <v>1.81</v>
+        <v>1.75</v>
       </c>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C14" s="5">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E14" s="1">
-        <v>61</v>
+        <v>56.3</v>
       </c>
       <c r="F14" s="1">
-        <v>1.66</v>
-      </c>
-      <c r="G14" s="1"/>
+        <v>1.65</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C15" s="5">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E15" s="1">
-        <v>51.5</v>
+        <v>71.3</v>
       </c>
       <c r="F15" s="1">
-        <v>1.69</v>
+        <v>1.81</v>
       </c>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C16" s="5">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E16" s="1">
-        <v>50.45</v>
+        <v>61</v>
       </c>
       <c r="F16" s="1">
-        <v>1.68</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>36</v>
-      </c>
+        <v>1.66</v>
+      </c>
+      <c r="G16" s="1"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C17" s="5">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="E17" s="1">
+        <v>51.5</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1.69</v>
+      </c>
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C18" s="5">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E18" s="1">
-        <v>53.4</v>
+        <v>50.45</v>
       </c>
       <c r="F18" s="1">
-        <v>1.69</v>
-      </c>
-      <c r="G18" s="1"/>
+        <v>1.68</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C19" s="5">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E19" s="1">
-        <v>72</v>
-      </c>
-      <c r="F19" s="1">
-        <v>1.8</v>
-      </c>
-      <c r="G19" s="1"/>
+        <v>26</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C20" s="5">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E20" s="1">
-        <v>87</v>
+        <v>53.4</v>
       </c>
       <c r="F20" s="1">
-        <v>1.79</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>42</v>
-      </c>
+        <v>1.69</v>
+      </c>
+      <c r="G20" s="1"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C21" s="5">
-        <v>84</v>
+        <v>38</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E21" s="1">
-        <v>73.400000000000006</v>
+        <v>72</v>
       </c>
       <c r="F21" s="1">
-        <v>1.67</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>44</v>
-      </c>
+        <v>1.8</v>
+      </c>
+      <c r="G21" s="1"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C22" s="5">
-        <v>73</v>
+        <v>34</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E22" s="1">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="F22" s="1">
-        <v>1.73</v>
-      </c>
-      <c r="G22" s="1"/>
+        <v>1.79</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C23" s="5">
-        <v>26</v>
+        <v>84</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E23" s="1">
-        <v>81.8</v>
+        <v>73.400000000000006</v>
       </c>
       <c r="F23" s="1">
-        <v>1.87</v>
-      </c>
-      <c r="G23" s="1"/>
+        <v>1.67</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C24" s="5">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="E24" s="1">
+        <v>73</v>
+      </c>
+      <c r="F24" s="1">
+        <v>1.73</v>
+      </c>
       <c r="G24" s="1"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C25" s="5">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E25" s="1">
-        <v>37.4</v>
+        <v>81.8</v>
       </c>
       <c r="F25" s="1">
-        <v>1.8</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>43</v>
-      </c>
+        <v>1.87</v>
+      </c>
+      <c r="G25" s="1"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C26" s="5">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E26" s="1">
-        <v>76.95</v>
-      </c>
-      <c r="F26" s="1">
-        <v>1.77</v>
-      </c>
-      <c r="G26" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C27" s="5">
-        <v>69</v>
+        <v>39</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
+        <v>30</v>
+      </c>
+      <c r="E27" s="1">
+        <v>37.4</v>
+      </c>
+      <c r="F27" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C28" s="5">
+        <v>43</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28" s="1">
+        <v>76.95</v>
+      </c>
+      <c r="F28" s="1">
+        <v>1.77</v>
+      </c>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="5">
+        <v>69</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="5">
         <v>48</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1" t="s">
+      <c r="D30" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B2:G28" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:G28">
-      <sortCondition ref="B2:B28"/>
+  <autoFilter ref="B2:G30" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:G30">
+      <sortCondition ref="B2:B30"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B10:G28">
-    <sortCondition ref="B10:B19"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B11:G30">
+    <sortCondition ref="B11:B21"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B3:B10" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Clearer folder structure. Correction in VSD_Subjects.xlsx
</commit_message>
<xml_diff>
--- a/MATLAB/res/VSD_Subjects.xlsx
+++ b/MATLAB/res/VSD_Subjects.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80BADD6A-9728-4791-BA84-63B9F36E9A0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F2438A-D3B5-41F1-81AA-4F12BE4428D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VSD_Subjects" sheetId="1" r:id="rId1"/>
@@ -15,16 +15,6 @@
     <definedName name="Sex" comment="White cell color: Sex was checked in the CT volume. Yellow cell color: Sex was taken from the metadata.">VSD_Subjects!$D$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -181,9 +171,6 @@
     <t>Duplicate of VSD z024 with conflicting metadata. Intraosseous access in the left tibia.</t>
   </si>
   <si>
-    <t>In the metadata the subject is incorrectly defined as female.</t>
-  </si>
-  <si>
     <t>Metacarpals are cut off and phalanges are missing. Volume data contains a lot of noise caused by metal artifacts.</t>
   </si>
   <si>
@@ -197,6 +184,9 @@
   </si>
   <si>
     <t>Spinal fusion of L4-L5-S1. Total hip replacement of the left and right hip joint. Total knee replacement of the right knee joint.</t>
+  </si>
+  <si>
+    <t>In the metadata the gender is specified as female while the biological sex visible in the CT data is male.</t>
   </si>
 </sst>
 </file>
@@ -295,9 +285,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -335,9 +325,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -370,26 +360,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -422,26 +395,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -972,7 +928,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
@@ -1028,7 +984,7 @@
         <v>1.79</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
@@ -1068,7 +1024,7 @@
         <v>1.73</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
@@ -1143,7 +1099,7 @@
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C30" s="5">
         <v>72</v>
@@ -1158,7 +1114,7 @@
         <v>1.72</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
@@ -1188,7 +1144,7 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>